<commit_message>
added 2 proportion test
</commit_message>
<xml_diff>
--- a/Statistics/hypothesis_testing_amy.xlsx
+++ b/Statistics/hypothesis_testing_amy.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00742989\ShareFile\Personal Folders\2019_Fall\BABI9010\week_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00742989\Desktop\Excel_fun\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015E52B1-E234-40D4-BBA6-1D2BA3C0B8E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="One_Sample_t_test" sheetId="1" r:id="rId1"/>
     <sheet name="one_sample_proportion_test" sheetId="3" r:id="rId2"/>
+    <sheet name="two_sample_proportion_test" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="70">
   <si>
     <t>One sample test for the mean</t>
   </si>
@@ -305,15 +307,33 @@
   <si>
     <t>Lookup Chart to Populate our test</t>
   </si>
+  <si>
+    <t>Two Sample Test for the Proportion</t>
+  </si>
+  <si>
+    <t>Sample 1</t>
+  </si>
+  <si>
+    <t>Sample 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypothesized Difference </t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>p1- p2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +362,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -382,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -496,11 +523,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -601,6 +643,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,7 +688,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -715,7 +774,13 @@
     <xdr:ext cx="65" cy="172227"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -774,7 +839,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -863,7 +934,13 @@
     <xdr:ext cx="65" cy="172227"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -917,7 +994,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -936,6 +1019,215 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0B662B-C8D2-463E-B696-4D718B63DE8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8389620" y="1752600"/>
+          <a:ext cx="2606040" cy="1508760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="15875" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1"/>
+            <a:t>Fill in the pale yellow squares! </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1"/>
+            <a:t>Select your test using the drop-down menu.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1"/>
+            <a:t> The</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
+            <a:t> rest of the chart will populate.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1"/>
+            <a:t>To see how valid this test is, check cell C20</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01357FA3-E276-46F0-A660-1D449FEA1FE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8389620" y="2381250"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200977</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>105808</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>392041</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>83058</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD0589A3-9FFF-41FD-9D82-753013D8184D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9428797" y="3649108"/>
+          <a:ext cx="6508044" cy="1272650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1205,7 +1497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1628,13 +1920,13 @@
     <mergeCell ref="E2:G3"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select from the menu" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select from the menu" sqref="C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$I$4:$I$6</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a whole number!" error="This is not a sample size!_x000a_" sqref="C5">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a whole number!" error="This is not a sample size!_x000a_" sqref="C5" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a probabiltiy!" error="This needs to be between 0 and 1" promptTitle="Alpha" prompt="Please enter a number between 0 and 1_x000a_" sqref="C9">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a probabiltiy!" error="This needs to be between 0 and 1" promptTitle="Alpha" prompt="Please enter a number between 0 and 1_x000a_" sqref="C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -1646,11 +1938,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2107,14 +2399,14 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$I$4:$I$6</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0</formula1>
       <formula2>C4</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="This needs to be between 0 and 1" promptTitle="Probability" prompt="This must be between 0 and 1" sqref="C7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="This needs to be between 0 and 1" promptTitle="Probability" prompt="This must be between 0 and 1" sqref="C7" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -2123,4 +2415,511 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F850BDB2-1477-4985-B172-30A65AC0D866}">
+  <dimension ref="B1:R24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" customWidth="1"/>
+    <col min="10" max="10" width="5.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="4.77734375" customWidth="1"/>
+    <col min="13" max="13" width="7.21875" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" s="31" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="G2" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
+      <c r="K2" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+    </row>
+    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="50"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
+      <c r="K3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="57">
+        <f>SUM(D4:E4)</f>
+        <v>400</v>
+      </c>
+      <c r="D4" s="56">
+        <v>200</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="5" t="str">
+        <f>CONCATENATE("H0: ",VLOOKUP($C$9,$K$4:$O$6,4,0))</f>
+        <v>H0: p1- p2 = 0</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="13" t="str">
+        <f>CONCATENATE($K$2, " ", L4, " ", $C$7)</f>
+        <v>p1- p2 = 0</v>
+      </c>
+      <c r="O4" s="13" t="str">
+        <f>CONCATENATE($K$2, " ", M4, " ", $C$7)</f>
+        <v>p1- p2 ≠ 0</v>
+      </c>
+      <c r="P4" s="13" t="str">
+        <f>CONCATENATE("z-test &lt; -", TEXT($C$12, "0.00"), " or z-test &gt; ",TEXT($C$12, "0.00"))</f>
+        <v>z-test &lt; -1.96 or z-test &gt; 1.96</v>
+      </c>
+      <c r="Q4" s="13">
+        <f>C16</f>
+        <v>1.2888239149881242E-2</v>
+      </c>
+      <c r="R4" s="6" t="str">
+        <f>IF(OR(C11&lt;-C12, C11&gt;C13), "REJECT", "FAIL TO REJECT")</f>
+        <v>REJECT</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="55">
+        <f>D5+E5</f>
+        <v>62</v>
+      </c>
+      <c r="D5" s="56">
+        <v>40</v>
+      </c>
+      <c r="E5" s="4">
+        <v>22</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="6" t="str">
+        <f>CONCATENATE("Ha: ",VLOOKUP($C$9,$K$4:$O$6,5,0))</f>
+        <v>Ha: p1- p2 ≠ 0</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="13" t="str">
+        <f>CONCATENATE($K$2, " ", L5, " ", $C$7)</f>
+        <v>p1- p2 ≥ 0</v>
+      </c>
+      <c r="O5" s="13" t="str">
+        <f>CONCATENATE(,$K$2, " ", M5, " ", $C$7)</f>
+        <v>p1- p2 &lt; 0</v>
+      </c>
+      <c r="P5" s="13" t="str">
+        <f>CONCATENATE("z-test &lt; -", TEXT($C$12, "0.00"))</f>
+        <v>z-test &lt; -1.96</v>
+      </c>
+      <c r="Q5" s="13">
+        <f>C17</f>
+        <v>6.444119574940621E-3</v>
+      </c>
+      <c r="R5" s="6" t="str">
+        <f t="shared" ref="R5:R6" si="0">IF(OR(C12&lt;-C13, C12&gt;C14), "REJECT", "FAIL TO REJECT")</f>
+        <v>REJECT</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="13">
+        <f>C5/C4</f>
+        <v>0.155</v>
+      </c>
+      <c r="D6" s="15">
+        <f>D5/D4</f>
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="7">
+        <f>E5/E4</f>
+        <v>0.11</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="6"/>
+      <c r="K6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="13" t="str">
+        <f>CONCATENATE($K$2, " ", L6, " ", $C$7)</f>
+        <v>p1- p2 ≤ 0</v>
+      </c>
+      <c r="O6" s="13" t="str">
+        <f>CONCATENATE($K$2, " ", M6, " ", $C$7)</f>
+        <v>p1- p2 &gt; 0</v>
+      </c>
+      <c r="P6" s="13" t="str">
+        <f>CONCATENATE("z-test &gt; ",TEXT($C$12, "0.00"))</f>
+        <v>z-test &gt; 1.96</v>
+      </c>
+      <c r="Q6" s="13">
+        <f>C17</f>
+        <v>6.444119574940621E-3</v>
+      </c>
+      <c r="R6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>REJECT</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="37">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="6" t="str">
+        <f>CONCATENATE(C9, " t-test of the proportion")</f>
+        <v>2-sided t-test of the proportion</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="7"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="6" t="str">
+        <f>CONCATENATE("α = ",C8)</f>
+        <v>α = 0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="33">
+        <f>(D6-E6-C7)/SQRT(C6*(1-C6)*(1/D4+1/E4))</f>
+        <v>2.4868426434476527</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="6" t="str">
+        <f>CONCATENATE("Reject H0 if ",VLOOKUP($C$9,K4:P6,6,0))</f>
+        <v>Reject H0 if z-test &lt; -1.96 or z-test &gt; 1.96</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="34">
+        <f>_xlfn.NORM.S.INV(1-C8/2)</f>
+        <v>1.9599639845400536</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="34">
+        <f>_xlfn.NORM.S.INV(1-C8)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="6" t="str">
+        <f>CONCATENATE("We have ", C5, " successes in ",C4, " trials")</f>
+        <v>We have 62 successes in 400 trials</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="34">
+        <f>-C13</f>
+        <v>-1.6448536269514715</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="C15" s="34"/>
+      <c r="G15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="6" t="str">
+        <f>CONCATENATE("The test statistic is z-test = ",TEXT($C$11,"0.00"))</f>
+        <v>The test statistic is z-test = 2.49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="34">
+        <f>2*C17</f>
+        <v>1.2888239149881242E-2</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="6" t="str">
+        <f>CONCATENATE("The p-value is ",TEXT(VLOOKUP($C$9,$K$4:$Q$6,7,0),"0.0000"))</f>
+        <v>The p-value is 0.0129</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="35">
+        <f>1-_xlfn.NORM.S.DIST(ABS(C11),1)</f>
+        <v>6.444119574940621E-3</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="24" t="str">
+        <f>IF(VLOOKUP($C$9,$K$4:$Q$6,7,0)&lt;C8, "REJECT", "FAIL TO REJECT")</f>
+        <v>REJECT</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="14"/>
+      <c r="H19" s="45" t="str">
+        <f>CONCATENATE("At the ",C8, " level of significance, there is ",IF(I18="REJECT"," ","not "), "enough evidence to show that ",VLOOKUP($C$9,$K$4:$O$6,5,0))</f>
+        <v>At the 0.05 level of significance, there is  enough evidence to show that p1- p2 ≠ 0</v>
+      </c>
+      <c r="I19" s="46"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="29" t="str">
+        <f>IF(COUNTIF(C21:C24, FALSE)=0,"VALID","NOT VALID!!")</f>
+        <v>VALID</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="6" t="b">
+        <f>IF(C5 &lt; 5, FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="6" t="b">
+        <f>IF((C4-C5) &lt; 5, FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="H19:I20"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="This needs to be between 0 and 1" promptTitle="Probability" prompt="This must be between 0 and 1" sqref="C7" xr:uid="{E7009662-68D7-42B1-B196-47E1B115F8D7}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{B7E86B2E-1C11-4B49-A0F4-71A84E397E5A}">
+      <formula1>0</formula1>
+      <formula2>C4</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{37AA8FF4-73D6-447E-8C94-1406C51E7973}">
+      <formula1>$K$4:$K$6</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected abs() error in p-value of single t-test
</commit_message>
<xml_diff>
--- a/Statistics/hypothesis_testing_amy.xlsx
+++ b/Statistics/hypothesis_testing_amy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00742989\Desktop\Excel_fun\Statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Desktop\Excel_fun\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEF1880-8A54-48F9-A718-0065390F9A76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28C70A5-8A24-4011-9CBD-5006D70A3575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="One_Sample_t_test" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1512,30 +1521,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.19921875" customWidth="1"/>
+    <col min="2" max="2" width="29.46484375" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="4" max="4" width="6.53125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="47.6640625" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" customWidth="1"/>
+    <col min="8" max="8" width="6.53125" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="4.77734375" customWidth="1"/>
-    <col min="11" max="11" width="7.21875" customWidth="1"/>
+    <col min="10" max="10" width="4.796875" customWidth="1"/>
+    <col min="11" max="11" width="7.19921875" customWidth="1"/>
     <col min="13" max="13" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B2" s="49" t="s">
         <v>0</v>
       </c>
@@ -1558,7 +1567,7 @@
       <c r="O2" s="47"/>
       <c r="P2" s="48"/>
     </row>
-    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="50" t="s">
         <v>48</v>
       </c>
@@ -1587,7 +1596,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E4" s="10" t="s">
         <v>27</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>FAIL TO REJECT</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B5" s="18" t="s">
         <v>1</v>
       </c>
@@ -1673,12 +1682,12 @@
         <v>REJECT</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
@@ -1713,7 +1722,7 @@
         <v>REJECT</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
@@ -1741,7 +1750,7 @@
       <c r="O7" s="16"/>
       <c r="P7" s="7"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
@@ -1752,7 +1761,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
@@ -1770,7 +1779,7 @@
         <v>α = 0.05</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
@@ -1781,7 +1790,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E11" s="12" t="s">
         <v>30</v>
       </c>
@@ -1793,19 +1802,19 @@
         <v>Reject H0 if t-test &lt; -2.07</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B12" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="5">
         <f>(C6-C8)/(C7/SQRT(C5))</f>
-        <v>1.6329931618554518</v>
+        <v>-1.6329931618554518</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
@@ -1821,10 +1830,10 @@
       </c>
       <c r="G13" s="6" t="str">
         <f>CONCATENATE("n = ",C5,", x̅ = ",TEXT(C6,"0.00"),", and s = ",TEXT(C7,"0.00"))</f>
-        <v>n = 24, x̅ = 9.00, and s = 3.00</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+        <v>n = 24, x̅ = 7.00, and s = 3.00</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B14" s="8" t="s">
         <v>13</v>
       </c>
@@ -1836,7 +1845,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="s">
         <v>12</v>
       </c>
@@ -1852,10 +1861,10 @@
       </c>
       <c r="G15" s="6" t="str">
         <f>CONCATENATE("The test statistic is ",TEXT($C$12,"0.00"))</f>
-        <v>The test statistic is 1.63</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+        <v>The test statistic is -1.63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B16" s="8"/>
       <c r="C16" s="6"/>
       <c r="E16" s="12"/>
@@ -1865,7 +1874,7 @@
         <v>The p-value is 0.0580</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="8" t="s">
         <v>15</v>
       </c>
@@ -1877,12 +1886,12 @@
       <c r="F17" s="13"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7">
-        <f>_xlfn.T.DIST.RT(C12,C5-1)</f>
+        <f>_xlfn.T.DIST.RT(ABS(C12),C5-1)</f>
         <v>5.8043508076162431E-2</v>
       </c>
       <c r="E18" s="12" t="s">
@@ -1896,7 +1905,7 @@
         <v>FAIL TO REJECT</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="E19" s="14"/>
       <c r="F19" s="52" t="str">
         <f>CONCATENATE("At the ",C9, " level of significance, there is ",IF(G18="REJECT"," ","not "), "enough evidence to show that ",VLOOKUP($C$10,$I$4:$M$6,5,0))</f>
@@ -1904,12 +1913,12 @@
       </c>
       <c r="G19" s="53"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="E20" s="14"/>
       <c r="F20" s="52"/>
       <c r="G20" s="53"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="E21" s="12" t="s">
         <v>45</v>
       </c>
@@ -1918,7 +1927,7 @@
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E22" s="15"/>
       <c r="F22" s="16"/>
       <c r="G22" s="7"/>
@@ -1957,29 +1966,29 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.19921875" customWidth="1"/>
+    <col min="2" max="2" width="29.46484375" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="4" max="4" width="6.1328125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="35.6640625" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" customWidth="1"/>
+    <col min="8" max="8" width="5.1328125" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="4.77734375" customWidth="1"/>
-    <col min="11" max="11" width="7.21875" customWidth="1"/>
+    <col min="10" max="10" width="4.796875" customWidth="1"/>
+    <col min="11" max="11" width="7.19921875" customWidth="1"/>
     <col min="13" max="13" width="7.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" customWidth="1"/>
+    <col min="16" max="16" width="10.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="31" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" s="31" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
       <c r="F1" s="32"/>
     </row>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="60" t="s">
         <v>61</v>
       </c>
@@ -2002,7 +2011,7 @@
       <c r="O2" s="47"/>
       <c r="P2" s="48"/>
     </row>
-    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E3" s="57"/>
       <c r="F3" s="58"/>
       <c r="G3" s="59"/>
@@ -2027,7 +2036,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
@@ -2074,7 +2083,7 @@
         <v>REJECT</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B5" s="8" t="s">
         <v>50</v>
       </c>
@@ -2119,7 +2128,7 @@
         <v>REJECT</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B6" s="8" t="s">
         <v>51</v>
       </c>
@@ -2160,7 +2169,7 @@
         <v>REJECT</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="8" t="s">
         <v>52</v>
       </c>
@@ -2188,7 +2197,7 @@
       <c r="O7" s="16"/>
       <c r="P7" s="7"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -2199,7 +2208,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
         <v>62</v>
       </c>
@@ -2217,12 +2226,12 @@
         <v>α = 0.06</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B11" s="18" t="s">
         <v>53</v>
       </c>
@@ -2241,7 +2250,7 @@
         <v>Reject H0 if z-test &lt; -1.88 or z-test &gt; 1.88</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
@@ -2253,7 +2262,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>13</v>
       </c>
@@ -2272,7 +2281,7 @@
         <v>We have 170 successes in 300 trials</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
@@ -2284,7 +2293,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B15" s="8"/>
       <c r="C15" s="34"/>
       <c r="E15" s="12" t="s">
@@ -2298,7 +2307,7 @@
         <v>The test statistic is z-test = 1.62</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
@@ -2313,7 +2322,7 @@
         <v>The p-value is 0.1057</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B17" s="9" t="s">
         <v>16</v>
       </c>
@@ -2325,7 +2334,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="E18" s="12" t="s">
         <v>35</v>
       </c>
@@ -2337,7 +2346,7 @@
         <v>FAIL TO REJECT</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E19" s="14"/>
       <c r="F19" s="52" t="str">
         <f>CONCATENATE("At the ",C8, " level of significance, there is ",IF(G18="REJECT"," ","not "), "enough evidence to show that ",VLOOKUP($C$9,$I$4:$M$6,5,0))</f>
@@ -2345,7 +2354,7 @@
       </c>
       <c r="G19" s="53"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B20" s="26" t="s">
         <v>54</v>
       </c>
@@ -2357,7 +2366,7 @@
       <c r="F20" s="52"/>
       <c r="G20" s="53"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="27" t="s">
         <v>59</v>
       </c>
@@ -2373,7 +2382,7 @@
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="27" t="s">
         <v>58</v>
       </c>
@@ -2385,7 +2394,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="27" t="s">
         <v>57</v>
       </c>
@@ -2394,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B24" s="28" t="s">
         <v>60</v>
       </c>
@@ -2433,35 +2442,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F850BDB2-1477-4985-B172-30A65AC0D866}">
   <dimension ref="B1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.19921875" customWidth="1"/>
+    <col min="2" max="2" width="29.46484375" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" customWidth="1"/>
+    <col min="5" max="5" width="9.46484375" customWidth="1"/>
+    <col min="6" max="6" width="4.86328125" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
     <col min="8" max="8" width="22.6640625" customWidth="1"/>
     <col min="9" max="9" width="35.6640625" customWidth="1"/>
-    <col min="10" max="10" width="5.109375" customWidth="1"/>
+    <col min="10" max="10" width="5.1328125" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="4.77734375" customWidth="1"/>
-    <col min="13" max="13" width="7.21875" customWidth="1"/>
+    <col min="12" max="12" width="4.796875" customWidth="1"/>
+    <col min="13" max="13" width="7.19921875" customWidth="1"/>
     <col min="15" max="15" width="7.6640625" customWidth="1"/>
-    <col min="18" max="18" width="10.5546875" customWidth="1"/>
+    <col min="18" max="18" width="10.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="31" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:18" s="31" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
       <c r="H1" s="32"/>
     </row>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="60" t="s">
         <v>64</v>
       </c>
@@ -2484,7 +2493,7 @@
       <c r="Q2" s="47"/>
       <c r="R2" s="48"/>
     </row>
-    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C3" s="45" t="s">
         <v>68</v>
       </c>
@@ -2518,7 +2527,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
@@ -2572,7 +2581,7 @@
         <v>REJECT</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B5" s="8" t="s">
         <v>50</v>
       </c>
@@ -2624,7 +2633,7 @@
         <v>REJECT</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="8" t="s">
         <v>51</v>
       </c>
@@ -2673,7 +2682,7 @@
         <v>REJECT</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
@@ -2701,7 +2710,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -2712,7 +2721,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
         <v>62</v>
       </c>
@@ -2730,12 +2739,12 @@
         <v>α = 0.05</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G10" s="12"/>
       <c r="H10" s="13"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B11" s="18" t="s">
         <v>53</v>
       </c>
@@ -2754,7 +2763,7 @@
         <v>Reject H0 if z-test &lt; -1.96 or z-test &gt; 1.96</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
@@ -2766,7 +2775,7 @@
       <c r="H12" s="13"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>13</v>
       </c>
@@ -2785,7 +2794,7 @@
         <v>1: We have 40 successes in 200 trials</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
@@ -2800,7 +2809,7 @@
         <v>2: We have 22 successes in 200 trials</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B15" s="8"/>
       <c r="C15" s="34"/>
       <c r="G15" s="12" t="s">
@@ -2814,7 +2823,7 @@
         <v>The test statistic is z-test = 2.49</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
@@ -2829,7 +2838,7 @@
         <v>The p-value is 0.0129</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B17" s="9" t="s">
         <v>16</v>
       </c>
@@ -2841,7 +2850,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G18" s="12" t="s">
         <v>35</v>
       </c>
@@ -2853,7 +2862,7 @@
         <v>REJECT</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="26" t="s">
         <v>54</v>
       </c>
@@ -2868,7 +2877,7 @@
       </c>
       <c r="I19" s="53"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B20" s="27" t="s">
         <v>70</v>
       </c>
@@ -2880,7 +2889,7 @@
       <c r="H20" s="52"/>
       <c r="I20" s="53"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B21" s="27" t="s">
         <v>71</v>
       </c>
@@ -2896,7 +2905,7 @@
       </c>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="27" t="s">
         <v>72</v>
       </c>
@@ -2908,7 +2917,7 @@
       <c r="H22" s="16"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="28" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
fixed error in t-test sheet with v-lookup
</commit_message>
<xml_diff>
--- a/Statistics/hypothesis_testing_amy.xlsx
+++ b/Statistics/hypothesis_testing_amy.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Desktop\Excel_fun\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D411C8-5B8C-4822-AEE4-6FC11D8C66E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E855E7-EF18-4D87-9E0B-B708EE9982C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="One_Sample_t_test" sheetId="1" r:id="rId1"/>
     <sheet name="one_sample_proportion_test" sheetId="3" r:id="rId2"/>
     <sheet name="two_sample_proportion_test" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1521,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1628,12 +1628,12 @@
       </c>
       <c r="N4" s="13" t="str">
         <f>"t-test &lt; -" &amp;TEXT($C$13, "0.00")&amp; " or t-test &gt; "&amp;TEXT($C$13, "0.00")</f>
-        <v>t-test &lt; -2.80 or t-test &gt; 2.80</v>
+        <v>t-test &lt; -3.89 or t-test &gt; 3.89</v>
       </c>
       <c r="O4" s="13"/>
       <c r="P4" s="13">
         <f>C17</f>
-        <v>1.1476844405111264E-15</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="6" t="str">
         <f>IF(OR(C12&lt;-C13, C12&gt;C14), "REJECT", "FAIL TO REJECT")</f>
@@ -1645,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>25</v>
+        <v>20000</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="13" t="s">
@@ -1674,12 +1674,12 @@
       </c>
       <c r="N5" s="13" t="str">
         <f>CONCATENATE("t-test &gt; ",TEXT($C$13, "0.00"))</f>
-        <v>t-test &gt; 2.80</v>
+        <v>t-test &gt; 3.89</v>
       </c>
       <c r="O5" s="13"/>
       <c r="P5" s="13">
         <f>C18</f>
-        <v>5.7384222025556319E-16</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="6" t="str">
         <f t="shared" ref="Q5:Q6" si="0">IF(OR(C13&lt;-C14, C13&gt;C15), "REJECT", "FAIL TO REJECT")</f>
@@ -1715,12 +1715,12 @@
       </c>
       <c r="N6" s="13" t="str">
         <f>CONCATENATE("t-test &gt; ",TEXT($C$13, "0.00"))</f>
-        <v>t-test &gt; 2.80</v>
+        <v>t-test &gt; 3.89</v>
       </c>
       <c r="O6" s="13"/>
       <c r="P6" s="13">
         <f>C18</f>
-        <v>5.7384222025556319E-16</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1772,7 +1772,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="4">
-        <v>0.01</v>
+        <v>1E-4</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>29</v>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="G9" s="6" t="str">
         <f>CONCATENATE("α = ",C9)</f>
-        <v>α = 0.01</v>
+        <v>α = 0.0001</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="G11" s="6" t="str">
         <f>CONCATENATE("Reject H0 if p &lt; ",C9," or if ",VLOOKUP($C$10,I4:N6,6,0),"")</f>
-        <v>Reject H0 if p &lt; 0.01 or if t-test &gt; 2.80</v>
+        <v>Reject H0 if p &lt; 0.0001 or if t-test &gt; 3.89</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.45">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="C12" s="5">
         <f>(C6-C8)/(C7/SQRT(C5))</f>
-        <v>-18.421052631578949</v>
+        <v>-521.02604929535084</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="C13" s="6">
         <f>_xlfn.T.INV.2T(C9,C5-1)</f>
-        <v>2.7969395047744556</v>
+        <v>3.8913768332777749</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>33</v>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="G13" s="6" t="str">
         <f>CONCATENATE("n = ",C5,", x̅ = ",TEXT(C6,"0.00"),", and s = ",TEXT(C7,"0.00"))</f>
-        <v>n = 25, x̅ = 13.50, and s = 0.95</v>
+        <v>n = 20000, x̅ = 13.50, and s = 0.95</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.45">
@@ -1845,7 +1845,7 @@
       </c>
       <c r="C14" s="6">
         <f>_xlfn.T.INV(1-C9,C5-1)</f>
-        <v>2.4921594731577557</v>
+        <v>3.7197060973714824</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="C15" s="6">
         <f>-C14</f>
-        <v>-2.4921594731577557</v>
+        <v>-3.7197060973714824</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>34</v>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="G15" s="6" t="str">
         <f>CONCATENATE("The test statistic is ",TEXT($C$12,"0.00"))</f>
-        <v>The test statistic is -18.42</v>
+        <v>The test statistic is -521.03</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.45">
@@ -1886,7 +1886,7 @@
       </c>
       <c r="C17" s="6">
         <f>2*C18</f>
-        <v>1.1476844405111264E-15</v>
+        <v>0</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="13"/>
@@ -1898,7 +1898,7 @@
       </c>
       <c r="C18" s="7">
         <f>_xlfn.T.DIST.RT(ABS(C12),C5-1)</f>
-        <v>5.7384222025556319E-16</v>
+        <v>0</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>35</v>
@@ -1907,7 +1907,7 @@
         <v>46</v>
       </c>
       <c r="G18" s="24" t="str">
-        <f>IF(VLOOKUP($C$10,$I$4:$P$6,7,0)&lt;C9, "REJECT", "FAIL TO REJECT")</f>
+        <f>IF(VLOOKUP($C$10,$I$4:$P$6,8,0)&lt;C9, "REJECT", "FAIL TO REJECT")</f>
         <v>REJECT</v>
       </c>
     </row>
@@ -1915,7 +1915,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="52" t="str">
         <f>CONCATENATE("At the ",C9, " level of significance, there is ",IF(G18="REJECT"," ","not "), "enough evidence to show that ",VLOOKUP($C$10,$I$4:$M$6,5,0))</f>
-        <v>At the 0.01 level of significance, there is  enough evidence to show that μ &lt; 17</v>
+        <v>At the 0.0001 level of significance, there is  enough evidence to show that μ &lt; 17</v>
       </c>
       <c r="G19" s="53"/>
     </row>
@@ -1968,8 +1968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2449,7 +2449,7 @@
   <dimension ref="B1:R23"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2539,13 +2539,13 @@
       </c>
       <c r="C4" s="42">
         <f>SUM(D4:E4)</f>
-        <v>400</v>
+        <v>198</v>
       </c>
       <c r="D4" s="41">
-        <v>200</v>
+        <v>103</v>
       </c>
       <c r="E4" s="4">
-        <v>200</v>
+        <v>95</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>27</v>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="I4" s="5" t="str">
         <f>CONCATENATE("H0: ",VLOOKUP($C$9,$K$4:$O$6,4,0))</f>
-        <v>H0: p1- p2 = 0.1</v>
+        <v>H0: p1- p2 ≤ 0</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>9</v>
@@ -2568,11 +2568,11 @@
       </c>
       <c r="N4" s="13" t="str">
         <f>CONCATENATE($K$2, " ", L4, " ", $C$7)</f>
-        <v>p1- p2 = 0.1</v>
+        <v>p1- p2 = 0</v>
       </c>
       <c r="O4" s="13" t="str">
         <f>CONCATENATE($K$2, " ", M4, " ", $C$7)</f>
-        <v>p1- p2 ≠ 0.1</v>
+        <v>p1- p2 ≠ 0</v>
       </c>
       <c r="P4" s="13" t="str">
         <f>CONCATENATE("z-test &lt; -", TEXT($C$12, "0.00"), " or z-test &gt; ",TEXT($C$12, "0.00"))</f>
@@ -2580,11 +2580,11 @@
       </c>
       <c r="Q4" s="13">
         <f>C16</f>
-        <v>0.78230548366097707</v>
+        <v>3.9131660055249817E-2</v>
       </c>
       <c r="R4" s="6" t="str">
         <f>IF(OR(C11&lt;-C12, C11&gt;C13), "REJECT", "FAIL TO REJECT")</f>
-        <v>FAIL TO REJECT</v>
+        <v>REJECT</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.45">
@@ -2593,13 +2593,13 @@
       </c>
       <c r="C5" s="40">
         <f>D5+E5</f>
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="D5" s="41">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="13" t="s">
@@ -2607,7 +2607,7 @@
       </c>
       <c r="I5" s="6" t="str">
         <f>CONCATENATE("Ha: ",VLOOKUP($C$9,$K$4:$O$6,5,0))</f>
-        <v>Ha: p1- p2 ≠ 0.1</v>
+        <v>Ha: p1- p2 &gt; 0</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>11</v>
@@ -2620,11 +2620,11 @@
       </c>
       <c r="N5" s="13" t="str">
         <f>CONCATENATE($K$2, " ", L5, " ", $C$7)</f>
-        <v>p1- p2 ≥ 0.1</v>
+        <v>p1- p2 ≥ 0</v>
       </c>
       <c r="O5" s="13" t="str">
         <f>CONCATENATE(,$K$2, " ", M5, " ", $C$7)</f>
-        <v>p1- p2 &lt; 0.1</v>
+        <v>p1- p2 &lt; 0</v>
       </c>
       <c r="P5" s="13" t="str">
         <f>CONCATENATE("z-test &lt; -", TEXT($C$12, "0.00"))</f>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="Q5" s="13">
         <f>C17</f>
-        <v>0.39115274183048854</v>
+        <v>1.9565830027624909E-2</v>
       </c>
       <c r="R5" s="6" t="str">
         <f t="shared" ref="R5:R6" si="0">IF(OR(C12&lt;-C13, C12&gt;C14), "REJECT", "FAIL TO REJECT")</f>
@@ -2645,15 +2645,15 @@
       </c>
       <c r="C6" s="13">
         <f>C5/C4</f>
-        <v>0.155</v>
+        <v>7.0707070707070704E-2</v>
       </c>
       <c r="D6" s="15">
         <f>D5/D4</f>
-        <v>0.2</v>
+        <v>0.10679611650485436</v>
       </c>
       <c r="E6" s="7">
         <f>E5/E4</f>
-        <v>0.11</v>
+        <v>3.1578947368421054E-2</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="13"/>
@@ -2669,11 +2669,11 @@
       </c>
       <c r="N6" s="13" t="str">
         <f>CONCATENATE($K$2, " ", L6, " ", $C$7)</f>
-        <v>p1- p2 ≤ 0.1</v>
+        <v>p1- p2 ≤ 0</v>
       </c>
       <c r="O6" s="13" t="str">
         <f>CONCATENATE($K$2, " ", M6, " ", $C$7)</f>
-        <v>p1- p2 &gt; 0.1</v>
+        <v>p1- p2 &gt; 0</v>
       </c>
       <c r="P6" s="13" t="str">
         <f>CONCATENATE("z-test &gt; ",TEXT($C$12, "0.00"))</f>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="Q6" s="13">
         <f>C17</f>
-        <v>0.39115274183048854</v>
+        <v>1.9565830027624909E-2</v>
       </c>
       <c r="R6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2693,7 +2693,7 @@
         <v>73</v>
       </c>
       <c r="C7" s="37">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>28</v>
@@ -2703,7 +2703,7 @@
       </c>
       <c r="I7" s="6" t="str">
         <f>CONCATENATE(C9, " t-test of the proportion")</f>
-        <v>2-sided t-test of the proportion</v>
+        <v>1-sided Right t-test of the proportion</v>
       </c>
       <c r="K7" s="22" t="s">
         <v>41</v>
@@ -2732,7 +2732,7 @@
         <v>62</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>29</v>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="C11" s="33">
         <f>(D6-E6-C7)/SQRT(C6*(1-C6)*(1/D4+1/E4))</f>
-        <v>-0.27631584927196123</v>
+        <v>2.0627997263783993</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>30</v>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="I11" s="6" t="str">
         <f>CONCATENATE("Reject H0 if ",VLOOKUP($C$9,K4:P6,6,0))</f>
-        <v>Reject H0 if z-test &lt; -1.96 or z-test &gt; 1.96</v>
+        <v>Reject H0 if z-test &gt; 1.96</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.45">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="I13" s="6" t="str">
         <f>CONCATENATE("1: We have ", D5, " successes in ",D4, " trials")</f>
-        <v>1: We have 40 successes in 200 trials</v>
+        <v>1: We have 11 successes in 103 trials</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.45">
@@ -2812,7 +2812,7 @@
       <c r="H14" s="13"/>
       <c r="I14" s="6" t="str">
         <f>CONCATENATE("2: We have ", E5, " successes in ",E4, " trials")</f>
-        <v>2: We have 22 successes in 200 trials</v>
+        <v>2: We have 3 successes in 95 trials</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.45">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="I15" s="6" t="str">
         <f>CONCATENATE("The test statistic is z-test = ",TEXT($C$11,"0.00"))</f>
-        <v>The test statistic is z-test = -0.28</v>
+        <v>The test statistic is z-test = 2.06</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.45">
@@ -2835,13 +2835,13 @@
       </c>
       <c r="C16" s="34">
         <f>2*C17</f>
-        <v>0.78230548366097707</v>
+        <v>3.9131660055249817E-2</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="13"/>
       <c r="I16" s="6" t="str">
         <f>CONCATENATE("The p-value is ",TEXT(VLOOKUP($C$9,$K$4:$Q$6,7,0),"0.0000"))</f>
-        <v>The p-value is 0.7823</v>
+        <v>The p-value is 0.0196</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="C17" s="35">
         <f>1-_xlfn.NORM.S.DIST(ABS(C11),1)</f>
-        <v>0.39115274183048854</v>
+        <v>1.9565830027624909E-2</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="13"/>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="I18" s="24" t="str">
         <f>IF(VLOOKUP($C$9,$K$4:$Q$6,7,0)&lt;C8, "REJECT", "FAIL TO REJECT")</f>
-        <v>FAIL TO REJECT</v>
+        <v>REJECT</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
@@ -2874,12 +2874,12 @@
       </c>
       <c r="C19" s="29" t="str">
         <f>IF(COUNTIF(C20:C23, FALSE)=0,"VALID","NOT VALID!!")</f>
-        <v>VALID</v>
+        <v>NOT VALID!!</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="52" t="str">
         <f>CONCATENATE("At the ",C8, " level of significance, there is ",IF(I18="REJECT"," ","not "), "enough evidence to show that ",VLOOKUP($C$9,$K$4:$O$6,5,0))</f>
-        <v>At the 0.05 level of significance, there is not enough evidence to show that p1- p2 ≠ 0.1</v>
+        <v>At the 0.05 level of significance, there is  enough evidence to show that p1- p2 &gt; 0</v>
       </c>
       <c r="I19" s="53"/>
     </row>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="C22" s="6" t="b">
         <f>IF(E5 &lt; 5, FALSE,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="16"/>

</xml_diff>